<commit_message>
fixes when superheating and subcooling start approaching zero in the optimization and changes gradient delta to 10**(-8)
</commit_message>
<xml_diff>
--- a/src/results/basic_exergy_efficiency.xlsx
+++ b/src/results/basic_exergy_efficiency.xlsx
@@ -1,26 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pflpe\Desktop\Projeto\projeto-final\src\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\repositories\projeto-final\src\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D07729A2-FBAA-4BB9-A8CE-139534B724A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EC68DEB-6E1F-4476-AE09-AF8A314BFF19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$73</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="30">
   <si>
     <t>refrigerant</t>
   </si>
@@ -59,12 +62,6 @@
   </si>
   <si>
     <t>default_exergy_efficiency</t>
-  </si>
-  <si>
-    <t>exergy_efficiency_components</t>
-  </si>
-  <si>
-    <t>default_exergy_efficiency_components</t>
   </si>
   <si>
     <t>R600a</t>
@@ -110,6 +107,12 @@
   </si>
   <si>
     <t>NH3</t>
+  </si>
+  <si>
+    <t>R404a</t>
+  </si>
+  <si>
+    <t>R410a</t>
   </si>
 </sst>
 </file>
@@ -472,28 +475,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O57"/>
+  <dimension ref="A1:M73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.1796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.36328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="26.90625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="34.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -533,22 +536,16 @@
       <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>15</v>
       </c>
       <c r="B2">
         <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D2">
         <v>256.93916246107642</v>
@@ -575,27 +572,21 @@
         <v>10.265616867181841</v>
       </c>
       <c r="L2">
-        <v>0.30459191249826267</v>
+        <v>0.30459191249826278</v>
       </c>
       <c r="M2">
-        <v>0.27919406743992747</v>
-      </c>
-      <c r="N2">
-        <v>0.30459191249826278</v>
-      </c>
-      <c r="O2">
         <v>0.27919406743992808</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B3">
         <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D3">
         <v>272.60193697697588</v>
@@ -627,22 +618,16 @@
       <c r="M3">
         <v>0.29604659812247408</v>
       </c>
-      <c r="N3">
-        <v>0.32334190999052997</v>
-      </c>
-      <c r="O3">
-        <v>0.29604659812247408</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B4">
         <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D4">
         <v>256.93916246107642</v>
@@ -669,27 +654,21 @@
         <v>10.265616867181841</v>
       </c>
       <c r="L4">
-        <v>0.30459191249826267</v>
+        <v>0.30459191249826278</v>
       </c>
       <c r="M4">
-        <v>0.27919406743992747</v>
-      </c>
-      <c r="N4">
-        <v>0.30459191249826278</v>
-      </c>
-      <c r="O4">
         <v>0.27919406743992808</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D5">
         <v>241.450158170864</v>
@@ -716,27 +695,21 @@
         <v>10.92415519617699</v>
       </c>
       <c r="L5">
-        <v>0.28330126987546328</v>
+        <v>0.28330126987546189</v>
       </c>
       <c r="M5">
-        <v>0.25996629737630089</v>
-      </c>
-      <c r="N5">
-        <v>0.28330126987546189</v>
-      </c>
-      <c r="O5">
         <v>0.25996629737629962</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B6">
         <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D6">
         <v>210.97110351317821</v>
@@ -763,27 +736,21 @@
         <v>12.50237096965861</v>
       </c>
       <c r="L6">
-        <v>0.23109442584484799</v>
+        <v>0.23109442584484849</v>
       </c>
       <c r="M6">
-        <v>0.21251692962193791</v>
-      </c>
-      <c r="N6">
-        <v>0.23109442584484849</v>
-      </c>
-      <c r="O6">
         <v>0.21251692962193869</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B7">
         <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D7">
         <v>210.97110351317821</v>
@@ -810,27 +777,21 @@
         <v>12.50237096965861</v>
       </c>
       <c r="L7">
-        <v>0.23109442584484799</v>
+        <v>0.23109442584484849</v>
       </c>
       <c r="M7">
-        <v>0.21251692962193791</v>
-      </c>
-      <c r="N7">
-        <v>0.23109442584484849</v>
-      </c>
-      <c r="O7">
         <v>0.21251692962193869</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B8">
         <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D8">
         <v>226.12927966124909</v>
@@ -857,27 +818,21 @@
         <v>11.66429665345103</v>
       </c>
       <c r="L8">
-        <v>0.25900040492600279</v>
+        <v>0.25900040492600329</v>
       </c>
       <c r="M8">
-        <v>0.23792547992760901</v>
-      </c>
-      <c r="N8">
-        <v>0.25900040492600329</v>
-      </c>
-      <c r="O8">
         <v>0.23792547992760929</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B9">
         <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D9">
         <v>241.450158170864</v>
@@ -904,27 +859,21 @@
         <v>10.92415519617699</v>
       </c>
       <c r="L9">
-        <v>0.28330126987546328</v>
+        <v>0.28330126987546189</v>
       </c>
       <c r="M9">
-        <v>0.25996629737630089</v>
-      </c>
-      <c r="N9">
-        <v>0.28330126987546189</v>
-      </c>
-      <c r="O9">
         <v>0.25996629737629962</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B10">
         <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D10">
         <v>261.25291779593078</v>
@@ -951,27 +900,21 @@
         <v>10.096113077903709</v>
       </c>
       <c r="L10">
-        <v>0.29930026628956402</v>
+        <v>0.29930026628956452</v>
       </c>
       <c r="M10">
-        <v>0.27458407147111907</v>
-      </c>
-      <c r="N10">
-        <v>0.29930026628956452</v>
-      </c>
-      <c r="O10">
         <v>0.27458407147111891</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B11">
         <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D11">
         <v>277.3602959287773</v>
@@ -998,27 +941,21 @@
         <v>9.5097929974711057</v>
       </c>
       <c r="L11">
-        <v>0.31748308808692077</v>
+        <v>0.3174830880869195</v>
       </c>
       <c r="M11">
-        <v>0.29096765928009499</v>
-      </c>
-      <c r="N11">
-        <v>0.3174830880869195</v>
-      </c>
-      <c r="O11">
         <v>0.2909676592800936</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B12">
         <v>29</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D12">
         <v>261.25291779593078</v>
@@ -1045,27 +982,21 @@
         <v>10.096113077903709</v>
       </c>
       <c r="L12">
-        <v>0.29930026628956402</v>
+        <v>0.29930026628956452</v>
       </c>
       <c r="M12">
-        <v>0.27458407147111907</v>
-      </c>
-      <c r="N12">
-        <v>0.29930026628956452</v>
-      </c>
-      <c r="O12">
         <v>0.27458407147111891</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B13">
         <v>28</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D13">
         <v>245.34774339893531</v>
@@ -1092,27 +1023,21 @@
         <v>10.75061446850645</v>
       </c>
       <c r="L13">
-        <v>0.27858714180997313</v>
+        <v>0.27858714180997451</v>
       </c>
       <c r="M13">
-        <v>0.25583648233739642</v>
-      </c>
-      <c r="N13">
-        <v>0.27858714180997451</v>
-      </c>
-      <c r="O13">
         <v>0.25583648233739598</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B14">
         <v>26</v>
       </c>
       <c r="C14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D14">
         <v>214.1155235061228</v>
@@ -1139,27 +1064,21 @@
         <v>12.31876585503421</v>
       </c>
       <c r="L14">
-        <v>0.2275788002138075</v>
+        <v>0.22757880021380739</v>
       </c>
       <c r="M14">
-        <v>0.20939598597712411</v>
-      </c>
-      <c r="N14">
-        <v>0.22757880021380739</v>
-      </c>
-      <c r="O14">
         <v>0.20939598597712461</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B15">
         <v>26</v>
       </c>
       <c r="C15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D15">
         <v>214.1155235061228</v>
@@ -1186,27 +1105,21 @@
         <v>12.31876585503421</v>
       </c>
       <c r="L15">
-        <v>0.2275788002138075</v>
+        <v>0.22757880021380739</v>
       </c>
       <c r="M15">
-        <v>0.20939598597712411</v>
-      </c>
-      <c r="N15">
-        <v>0.22757880021380739</v>
-      </c>
-      <c r="O15">
         <v>0.20939598597712461</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B16">
         <v>27</v>
       </c>
       <c r="C16" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D16">
         <v>229.63757024273289</v>
@@ -1233,27 +1146,21 @@
         <v>11.48609522915587</v>
       </c>
       <c r="L16">
-        <v>0.25487706822268952</v>
+        <v>0.25487706822269102</v>
       </c>
       <c r="M16">
-        <v>0.23429057071200141</v>
-      </c>
-      <c r="N16">
-        <v>0.25487706822269102</v>
-      </c>
-      <c r="O16">
         <v>0.23429057071200121</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B17">
         <v>28</v>
       </c>
       <c r="C17" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D17">
         <v>245.34774339893531</v>
@@ -1280,27 +1187,21 @@
         <v>10.75061446850645</v>
       </c>
       <c r="L17">
-        <v>0.27858714180997313</v>
+        <v>0.27858714180997451</v>
       </c>
       <c r="M17">
-        <v>0.25583648233739642</v>
-      </c>
-      <c r="N17">
-        <v>0.27858714180997451</v>
-      </c>
-      <c r="O17">
         <v>0.25583648233739598</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B18">
         <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D18">
         <v>268.02730400533193</v>
@@ -1327,27 +1228,21 @@
         <v>9.8409339667406783</v>
       </c>
       <c r="L18">
-        <v>0.29972471480849477</v>
+        <v>0.2997247148084955</v>
       </c>
       <c r="M18">
-        <v>0.26764396305941002</v>
-      </c>
-      <c r="N18">
-        <v>0.2997247148084955</v>
-      </c>
-      <c r="O18">
         <v>0.26764396305941102</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B19">
         <v>30</v>
       </c>
       <c r="C19" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D19">
         <v>284.96741346792072</v>
@@ -1374,27 +1269,21 @@
         <v>9.2559319955259518</v>
       </c>
       <c r="L19">
-        <v>0.31774017625758633</v>
+        <v>0.31774017625758622</v>
       </c>
       <c r="M19">
-        <v>0.28320036702272172</v>
-      </c>
-      <c r="N19">
-        <v>0.31774017625758622</v>
-      </c>
-      <c r="O19">
         <v>0.283200367022722</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B20">
         <v>29</v>
       </c>
       <c r="C20" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D20">
         <v>268.02730400533193</v>
@@ -1421,27 +1310,21 @@
         <v>9.8409339667406783</v>
       </c>
       <c r="L20">
-        <v>0.29972471480849477</v>
+        <v>0.2997247148084955</v>
       </c>
       <c r="M20">
-        <v>0.26764396305941002</v>
-      </c>
-      <c r="N20">
-        <v>0.2997247148084955</v>
-      </c>
-      <c r="O20">
         <v>0.26764396305941102</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B21">
         <v>28</v>
       </c>
       <c r="C21" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D21">
         <v>251.35531095124119</v>
@@ -1468,27 +1351,21 @@
         <v>10.493667271314029</v>
       </c>
       <c r="L21">
-        <v>0.27914539154911178</v>
+        <v>0.279145391549112</v>
       </c>
       <c r="M21">
-        <v>0.24972181165799159</v>
-      </c>
-      <c r="N21">
-        <v>0.279145391549112</v>
-      </c>
-      <c r="O21">
         <v>0.24972181165799209</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B22">
         <v>26</v>
       </c>
       <c r="C22" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D22">
         <v>218.77148213955641</v>
@@ -1515,27 +1392,21 @@
         <v>12.05659427912741</v>
       </c>
       <c r="L22">
-        <v>0.22828638654824271</v>
+        <v>0.2282863865482434</v>
       </c>
       <c r="M22">
-        <v>0.2049395593936327</v>
-      </c>
-      <c r="N22">
-        <v>0.2282863865482434</v>
-      </c>
-      <c r="O22">
         <v>0.20493955939363229</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B23">
         <v>26</v>
       </c>
       <c r="C23" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D23">
         <v>218.77148213955641</v>
@@ -1562,27 +1433,21 @@
         <v>12.05659427912741</v>
       </c>
       <c r="L23">
-        <v>0.22828638654824271</v>
+        <v>0.2282863865482434</v>
       </c>
       <c r="M23">
-        <v>0.2049395593936327</v>
-      </c>
-      <c r="N23">
-        <v>0.2282863865482434</v>
-      </c>
-      <c r="O23">
         <v>0.20493955939363229</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B24">
         <v>27</v>
       </c>
       <c r="C24" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D24">
         <v>234.9402388622556</v>
@@ -1609,27 +1474,21 @@
         <v>11.226850763297451</v>
       </c>
       <c r="L24">
-        <v>0.25553143963225938</v>
+        <v>0.25553143963225988</v>
       </c>
       <c r="M24">
-        <v>0.22900256528908619</v>
-      </c>
-      <c r="N24">
-        <v>0.25553143963225988</v>
-      </c>
-      <c r="O24">
         <v>0.229002565289086</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B25">
         <v>28</v>
       </c>
       <c r="C25" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D25">
         <v>251.35531095124119</v>
@@ -1656,27 +1515,21 @@
         <v>10.493667271314029</v>
       </c>
       <c r="L25">
-        <v>0.27914539154911178</v>
+        <v>0.279145391549112</v>
       </c>
       <c r="M25">
-        <v>0.24972181165799159</v>
-      </c>
-      <c r="N25">
-        <v>0.279145391549112</v>
-      </c>
-      <c r="O25">
         <v>0.24972181165799209</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B26">
         <v>29</v>
       </c>
       <c r="C26" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D26">
         <v>260.95930273577608</v>
@@ -1703,27 +1556,21 @@
         <v>10.10747259188777</v>
       </c>
       <c r="L26">
-        <v>0.30229563793871772</v>
+        <v>0.30229563793871872</v>
       </c>
       <c r="M26">
-        <v>0.27489301626755802</v>
-      </c>
-      <c r="N26">
-        <v>0.30229563793871872</v>
-      </c>
-      <c r="O26">
         <v>0.27489301626755841</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B27">
         <v>30</v>
       </c>
       <c r="C27" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D27">
         <v>277.08583091778752</v>
@@ -1750,27 +1597,21 @@
         <v>9.5192128419680841</v>
       </c>
       <c r="L27">
-        <v>0.32072053726681538</v>
+        <v>0.32072053726681621</v>
       </c>
       <c r="M27">
-        <v>0.29125587481799342</v>
-      </c>
-      <c r="N27">
-        <v>0.32072053726681621</v>
-      </c>
-      <c r="O27">
         <v>0.2912558748179942</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B28">
         <v>29</v>
       </c>
       <c r="C28" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D28">
         <v>260.95930273577608</v>
@@ -1797,27 +1638,21 @@
         <v>10.10747259188777</v>
       </c>
       <c r="L28">
-        <v>0.30229563793871772</v>
+        <v>0.30229563793871872</v>
       </c>
       <c r="M28">
-        <v>0.27489301626755802</v>
-      </c>
-      <c r="N28">
-        <v>0.30229563793871872</v>
-      </c>
-      <c r="O28">
         <v>0.27489301626755841</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B29">
         <v>28</v>
       </c>
       <c r="C29" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D29">
         <v>245.03962018009719</v>
@@ -1844,27 +1679,21 @@
         <v>10.764132747436561</v>
       </c>
       <c r="L29">
-        <v>0.28132343201791721</v>
+        <v>0.28132343201791699</v>
       </c>
       <c r="M29">
-        <v>0.25615818198897128</v>
-      </c>
-      <c r="N29">
-        <v>0.28132343201791699</v>
-      </c>
-      <c r="O29">
         <v>0.25615818198897022</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B30">
         <v>26</v>
       </c>
       <c r="C30" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D30">
         <v>213.79165634544279</v>
@@ -1891,27 +1720,21 @@
         <v>12.337427218104921</v>
       </c>
       <c r="L30">
-        <v>0.22973159162684881</v>
+        <v>0.22973159162684781</v>
       </c>
       <c r="M30">
-        <v>0.20971319425641549</v>
-      </c>
-      <c r="N30">
-        <v>0.22973159162684781</v>
-      </c>
-      <c r="O30">
         <v>0.2097131942564173</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B31">
         <v>26</v>
       </c>
       <c r="C31" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D31">
         <v>213.79165634544279</v>
@@ -1938,27 +1761,21 @@
         <v>12.337427218104921</v>
       </c>
       <c r="L31">
-        <v>0.22973159162684881</v>
+        <v>0.22973159162684781</v>
       </c>
       <c r="M31">
-        <v>0.20971319425641549</v>
-      </c>
-      <c r="N31">
-        <v>0.22973159162684781</v>
-      </c>
-      <c r="O31">
         <v>0.2097131942564173</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B32">
         <v>27</v>
       </c>
       <c r="C32" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D32">
         <v>229.31941754568479</v>
@@ -1985,27 +1802,21 @@
         <v>11.50203078408976</v>
       </c>
       <c r="L32">
-        <v>0.25733390872903128</v>
+        <v>0.25733390872903211</v>
       </c>
       <c r="M32">
-        <v>0.23461562027720059</v>
-      </c>
-      <c r="N32">
-        <v>0.25733390872903211</v>
-      </c>
-      <c r="O32">
         <v>0.23461562027719829</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B33">
         <v>28</v>
       </c>
       <c r="C33" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D33">
         <v>245.03962018009719</v>
@@ -2032,27 +1843,21 @@
         <v>10.764132747436561</v>
       </c>
       <c r="L33">
-        <v>0.28132343201791721</v>
+        <v>0.28132343201791699</v>
       </c>
       <c r="M33">
-        <v>0.25615818198897128</v>
-      </c>
-      <c r="N33">
-        <v>0.28132343201791699</v>
-      </c>
-      <c r="O33">
         <v>0.25615818198897022</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B34">
         <v>29</v>
       </c>
       <c r="C34" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D34">
         <v>262.55266687281971</v>
@@ -2079,27 +1884,21 @@
         <v>10.046132958450089</v>
       </c>
       <c r="L34">
-        <v>0.29385555170434852</v>
+        <v>0.29385555170434863</v>
       </c>
       <c r="M34">
-        <v>0.27322476174605032</v>
-      </c>
-      <c r="N34">
-        <v>0.29385555170434863</v>
-      </c>
-      <c r="O34">
         <v>0.27322476174605009</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B35">
         <v>30</v>
       </c>
       <c r="C35" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D35">
         <v>278.63776256438268</v>
@@ -2126,27 +1925,21 @@
         <v>9.4661935831132755</v>
       </c>
       <c r="L35">
-        <v>0.31175783223946979</v>
+        <v>0.31175783223947012</v>
       </c>
       <c r="M35">
-        <v>0.28963366394023282</v>
-      </c>
-      <c r="N35">
-        <v>0.31175783223947012</v>
-      </c>
-      <c r="O35">
         <v>0.28963366394023271</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B36">
         <v>29</v>
       </c>
       <c r="C36" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D36">
         <v>262.55266687281971</v>
@@ -2173,27 +1966,21 @@
         <v>10.046132958450089</v>
       </c>
       <c r="L36">
-        <v>0.29385555170434852</v>
+        <v>0.29385555170434863</v>
       </c>
       <c r="M36">
-        <v>0.27322476174605032</v>
-      </c>
-      <c r="N36">
-        <v>0.29385555170434863</v>
-      </c>
-      <c r="O36">
         <v>0.27322476174605009</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B37">
         <v>28</v>
       </c>
       <c r="C37" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D37">
         <v>246.65393467072661</v>
@@ -2220,27 +2007,21 @@
         <v>10.693683048361439</v>
       </c>
       <c r="L37">
-        <v>0.2734794159616607</v>
+        <v>0.27347941596166081</v>
       </c>
       <c r="M37">
-        <v>0.25448166356800989</v>
-      </c>
-      <c r="N37">
-        <v>0.27347941596166081</v>
-      </c>
-      <c r="O37">
         <v>0.25448166356800961</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B38">
         <v>26</v>
       </c>
       <c r="C38" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D38">
         <v>215.39202257749611</v>
@@ -2267,27 +2048,21 @@
         <v>12.24575993315166</v>
       </c>
       <c r="L38">
-        <v>0.223351390888719</v>
+        <v>0.22335139088871819</v>
       </c>
       <c r="M38">
-        <v>0.20815502181117901</v>
-      </c>
-      <c r="N38">
-        <v>0.22335139088871819</v>
-      </c>
-      <c r="O38">
         <v>0.20815502181117851</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B39">
         <v>26</v>
       </c>
       <c r="C39" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D39">
         <v>215.39202257749611</v>
@@ -2314,27 +2089,21 @@
         <v>12.24575993315166</v>
       </c>
       <c r="L39">
-        <v>0.223351390888719</v>
+        <v>0.22335139088871819</v>
       </c>
       <c r="M39">
-        <v>0.20815502181117901</v>
-      </c>
-      <c r="N39">
-        <v>0.22335139088871819</v>
-      </c>
-      <c r="O39">
         <v>0.20815502181117851</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B40">
         <v>27</v>
       </c>
       <c r="C40" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D40">
         <v>230.93561542980751</v>
@@ -2361,27 +2130,21 @@
         <v>11.4215340716976</v>
       </c>
       <c r="L40">
-        <v>0.25017144502751559</v>
+        <v>0.25017144502751598</v>
       </c>
       <c r="M40">
-        <v>0.23297366795915561</v>
-      </c>
-      <c r="N40">
-        <v>0.25017144502751598</v>
-      </c>
-      <c r="O40">
         <v>0.2329736679591565</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B41">
         <v>28</v>
       </c>
       <c r="C41" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D41">
         <v>246.65393467072661</v>
@@ -2408,27 +2171,21 @@
         <v>10.693683048361439</v>
       </c>
       <c r="L41">
-        <v>0.2734794159616607</v>
+        <v>0.27347941596166081</v>
       </c>
       <c r="M41">
-        <v>0.25448166356800989</v>
-      </c>
-      <c r="N41">
-        <v>0.27347941596166081</v>
-      </c>
-      <c r="O41">
         <v>0.25448166356800961</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B42">
         <v>29</v>
       </c>
       <c r="C42" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D42">
         <v>265.78105254805217</v>
@@ -2455,27 +2212,21 @@
         <v>9.9241047272289116</v>
       </c>
       <c r="L42">
-        <v>0.29458927608272611</v>
+        <v>0.29458927608272689</v>
       </c>
       <c r="M42">
-        <v>0.26990595892514457</v>
-      </c>
-      <c r="N42">
-        <v>0.29458927608272689</v>
-      </c>
-      <c r="O42">
         <v>0.26990595892514552</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B43">
         <v>30</v>
       </c>
       <c r="C43" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D43">
         <v>282.2679374950132</v>
@@ -2502,27 +2253,21 @@
         <v>9.3444513160358458</v>
       </c>
       <c r="L43">
-        <v>0.31241531773953352</v>
+        <v>0.31241531773953479</v>
       </c>
       <c r="M43">
-        <v>0.28590876030706308</v>
-      </c>
-      <c r="N43">
-        <v>0.31241531773953479</v>
-      </c>
-      <c r="O43">
         <v>0.28590876030706391</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B44">
         <v>29</v>
       </c>
       <c r="C44" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D44">
         <v>265.78105254805217</v>
@@ -2549,27 +2294,21 @@
         <v>9.9241047272289116</v>
       </c>
       <c r="L44">
-        <v>0.29458927608272611</v>
+        <v>0.29458927608272689</v>
       </c>
       <c r="M44">
-        <v>0.26990595892514457</v>
-      </c>
-      <c r="N44">
-        <v>0.29458927608272689</v>
-      </c>
-      <c r="O44">
         <v>0.26990595892514552</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B45">
         <v>28</v>
       </c>
       <c r="C45" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D45">
         <v>249.51483350340041</v>
@@ -2596,27 +2335,21 @@
         <v>10.571070917769919</v>
       </c>
       <c r="L45">
-        <v>0.2742618002773336</v>
+        <v>0.27426180027733188</v>
       </c>
       <c r="M45">
-        <v>0.2515638158231836</v>
-      </c>
-      <c r="N45">
-        <v>0.27426180027733188</v>
-      </c>
-      <c r="O45">
         <v>0.2515638158231841</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B46">
         <v>26</v>
       </c>
       <c r="C46" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D46">
         <v>217.6115260008979</v>
@@ -2643,27 +2376,21 @@
         <v>12.120860730461111</v>
       </c>
       <c r="L46">
-        <v>0.22413740607380631</v>
+        <v>0.22413740607380681</v>
       </c>
       <c r="M46">
-        <v>0.2060319689012598</v>
-      </c>
-      <c r="N46">
-        <v>0.22413740607380681</v>
-      </c>
-      <c r="O46">
         <v>0.20603196890125919</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B47">
         <v>26</v>
       </c>
       <c r="C47" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D47">
         <v>217.6115260008979</v>
@@ -2690,27 +2417,21 @@
         <v>12.120860730461111</v>
       </c>
       <c r="L47">
-        <v>0.22413740607380631</v>
+        <v>0.22413740607380681</v>
       </c>
       <c r="M47">
-        <v>0.2060319689012598</v>
-      </c>
-      <c r="N47">
-        <v>0.22413740607380681</v>
-      </c>
-      <c r="O47">
         <v>0.20603196890125919</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B48">
         <v>27</v>
       </c>
       <c r="C48" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D48">
         <v>233.46096374415879</v>
@@ -2740,24 +2461,18 @@
         <v>0.25097235251371519</v>
       </c>
       <c r="M48">
-        <v>0.230453590725543</v>
-      </c>
-      <c r="N48">
-        <v>0.25097235251371519</v>
-      </c>
-      <c r="O48">
         <v>0.2304535907255425</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B49">
         <v>28</v>
       </c>
       <c r="C49" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D49">
         <v>249.51483350340041</v>
@@ -2784,27 +2499,21 @@
         <v>10.571070917769919</v>
       </c>
       <c r="L49">
-        <v>0.2742618002773336</v>
+        <v>0.27426180027733188</v>
       </c>
       <c r="M49">
-        <v>0.2515638158231836</v>
-      </c>
-      <c r="N49">
-        <v>0.27426180027733188</v>
-      </c>
-      <c r="O49">
         <v>0.2515638158231841</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B50">
         <v>29</v>
       </c>
       <c r="C50" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D50">
         <v>253.8941088168996</v>
@@ -2831,27 +2540,21 @@
         <v>10.38873651811347</v>
       </c>
       <c r="L50">
-        <v>0.29473308041479279</v>
+        <v>0.29473308041479268</v>
       </c>
       <c r="M50">
-        <v>0.28254255361178909</v>
-      </c>
-      <c r="N50">
-        <v>0.29473308041479268</v>
-      </c>
-      <c r="O50">
         <v>0.28254255361178893</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B51">
         <v>30</v>
       </c>
       <c r="C51" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D51">
         <v>269.08341429201039</v>
@@ -2878,27 +2581,21 @@
         <v>9.8023098411321001</v>
       </c>
       <c r="L51">
-        <v>0.31294018644563831</v>
+        <v>0.3129401864456377</v>
       </c>
       <c r="M51">
-        <v>0.29991769019272108</v>
-      </c>
-      <c r="N51">
-        <v>0.3129401864456377</v>
-      </c>
-      <c r="O51">
         <v>0.29991769019272141</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B52">
         <v>29</v>
       </c>
       <c r="C52" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D52">
         <v>253.8941088168996</v>
@@ -2925,27 +2622,21 @@
         <v>10.38873651811347</v>
       </c>
       <c r="L52">
-        <v>0.29473308041479279</v>
+        <v>0.29473308041479268</v>
       </c>
       <c r="M52">
-        <v>0.28254255361178909</v>
-      </c>
-      <c r="N52">
-        <v>0.29473308041479268</v>
-      </c>
-      <c r="O52">
         <v>0.28254255361178893</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B53">
         <v>28</v>
       </c>
       <c r="C53" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D53">
         <v>238.8279872823953</v>
@@ -2972,27 +2663,21 @@
         <v>11.044095082881549</v>
       </c>
       <c r="L53">
-        <v>0.2740892248142055</v>
+        <v>0.27408922481420472</v>
       </c>
       <c r="M53">
-        <v>0.26282055271178267</v>
-      </c>
-      <c r="N53">
-        <v>0.27408922481420472</v>
-      </c>
-      <c r="O53">
         <v>0.26282055271178212</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B54">
         <v>26</v>
       </c>
       <c r="C54" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D54">
         <v>209.0581079005274</v>
@@ -3019,27 +2704,21 @@
         <v>12.61677447714691</v>
       </c>
       <c r="L54">
-        <v>0.22354386580053831</v>
+        <v>0.22354386580053581</v>
       </c>
       <c r="M54">
-        <v>0.21446157533821031</v>
-      </c>
-      <c r="N54">
-        <v>0.22354386580053581</v>
-      </c>
-      <c r="O54">
         <v>0.21446157533820709</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B55">
         <v>26</v>
       </c>
       <c r="C55" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D55">
         <v>209.0581079005274</v>
@@ -3066,27 +2745,21 @@
         <v>12.61677447714691</v>
       </c>
       <c r="L55">
-        <v>0.22354386580053831</v>
+        <v>0.22354386580053581</v>
       </c>
       <c r="M55">
-        <v>0.21446157533821031</v>
-      </c>
-      <c r="N55">
-        <v>0.22354386580053581</v>
-      </c>
-      <c r="O55">
         <v>0.21446157533820709</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B56">
         <v>27</v>
       </c>
       <c r="C56" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D56">
         <v>223.88323842519969</v>
@@ -3113,27 +2786,21 @@
         <v>11.781315200517991</v>
       </c>
       <c r="L56">
-        <v>0.25055221287803958</v>
+        <v>0.25055221287803742</v>
       </c>
       <c r="M56">
-        <v>0.24031239572703711</v>
-      </c>
-      <c r="N56">
-        <v>0.25055221287803742</v>
-      </c>
-      <c r="O56">
         <v>0.240312395727038</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B57">
         <v>28</v>
       </c>
       <c r="C57" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D57">
         <v>238.8279872823953</v>
@@ -3160,19 +2827,670 @@
         <v>11.044095082881549</v>
       </c>
       <c r="L57">
-        <v>0.2740892248142055</v>
+        <v>0.27408922481420472</v>
       </c>
       <c r="M57">
-        <v>0.26282055271178267</v>
-      </c>
-      <c r="N57">
-        <v>0.27408922481420472</v>
-      </c>
-      <c r="O57">
         <v>0.26282055271178212</v>
       </c>
     </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>28</v>
+      </c>
+      <c r="B58">
+        <v>29</v>
+      </c>
+      <c r="C58" t="s">
+        <v>14</v>
+      </c>
+      <c r="D58">
+        <v>287.2485047300741</v>
+      </c>
+      <c r="E58">
+        <v>68.939641135217784</v>
+      </c>
+      <c r="F58">
+        <v>47.844110947841138</v>
+      </c>
+      <c r="G58">
+        <v>2975.517826568373</v>
+      </c>
+      <c r="H58">
+        <v>10</v>
+      </c>
+      <c r="I58">
+        <v>0</v>
+      </c>
+      <c r="J58">
+        <v>10.35868865310352</v>
+      </c>
+      <c r="K58">
+        <v>9.1824289998605053</v>
+      </c>
+      <c r="L58">
+        <v>0.28172534157684159</v>
+      </c>
+      <c r="M58">
+        <v>0.24973459799042749</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>28</v>
+      </c>
+      <c r="B59">
+        <v>30</v>
+      </c>
+      <c r="C59" t="s">
+        <v>15</v>
+      </c>
+      <c r="D59">
+        <v>305.59572097303561</v>
+      </c>
+      <c r="E59">
+        <v>73.342973033528537</v>
+      </c>
+      <c r="F59">
+        <v>50.900023285268809</v>
+      </c>
+      <c r="G59">
+        <v>2982.1434925025528</v>
+      </c>
+      <c r="H59">
+        <v>10</v>
+      </c>
+      <c r="I59">
+        <v>0</v>
+      </c>
+      <c r="J59">
+        <v>9.7584595851251592</v>
+      </c>
+      <c r="K59">
+        <v>8.6311385238039158</v>
+      </c>
+      <c r="L59">
+        <v>0.29857601994263677</v>
+      </c>
+      <c r="M59">
+        <v>0.264083789611542</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>28</v>
+      </c>
+      <c r="B60">
+        <v>29</v>
+      </c>
+      <c r="C60" t="s">
+        <v>16</v>
+      </c>
+      <c r="D60">
+        <v>287.2485047300741</v>
+      </c>
+      <c r="E60">
+        <v>68.939641135217784</v>
+      </c>
+      <c r="F60">
+        <v>47.844110947841138</v>
+      </c>
+      <c r="G60">
+        <v>2975.517826568373</v>
+      </c>
+      <c r="H60">
+        <v>10</v>
+      </c>
+      <c r="I60">
+        <v>0</v>
+      </c>
+      <c r="J60">
+        <v>10.35868865310352</v>
+      </c>
+      <c r="K60">
+        <v>9.1824289998605053</v>
+      </c>
+      <c r="L60">
+        <v>0.28172534157684159</v>
+      </c>
+      <c r="M60">
+        <v>0.24973459799042749</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>28</v>
+      </c>
+      <c r="B61">
+        <v>28</v>
+      </c>
+      <c r="C61" t="s">
+        <v>17</v>
+      </c>
+      <c r="D61">
+        <v>269.27503525084558</v>
+      </c>
+      <c r="E61">
+        <v>64.626008460202939</v>
+      </c>
+      <c r="F61">
+        <v>44.850449871380832</v>
+      </c>
+      <c r="G61">
+        <v>2969.1648750043551</v>
+      </c>
+      <c r="H61">
+        <v>10</v>
+      </c>
+      <c r="I61">
+        <v>0</v>
+      </c>
+      <c r="J61">
+        <v>11.02651373618205</v>
+      </c>
+      <c r="K61">
+        <v>9.7953343411240628</v>
+      </c>
+      <c r="L61">
+        <v>0.26240216268323718</v>
+      </c>
+      <c r="M61">
+        <v>0.2331033159539968</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>28</v>
+      </c>
+      <c r="B62">
+        <v>26</v>
+      </c>
+      <c r="C62" t="s">
+        <v>18</v>
+      </c>
+      <c r="D62">
+        <v>234.37229599366921</v>
+      </c>
+      <c r="E62">
+        <v>56.249351038480597</v>
+      </c>
+      <c r="F62">
+        <v>39.037049620705531</v>
+      </c>
+      <c r="G62">
+        <v>2957.210354943496</v>
+      </c>
+      <c r="H62">
+        <v>10</v>
+      </c>
+      <c r="I62">
+        <v>0</v>
+      </c>
+      <c r="J62">
+        <v>12.61757641792004</v>
+      </c>
+      <c r="K62">
+        <v>11.254056239101089</v>
+      </c>
+      <c r="L62">
+        <v>0.21447520683188909</v>
+      </c>
+      <c r="M62">
+        <v>0.1912979132942568</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>28</v>
+      </c>
+      <c r="B63">
+        <v>26</v>
+      </c>
+      <c r="C63" t="s">
+        <v>19</v>
+      </c>
+      <c r="D63">
+        <v>234.37229599366921</v>
+      </c>
+      <c r="E63">
+        <v>56.249351038480597</v>
+      </c>
+      <c r="F63">
+        <v>39.037049620705531</v>
+      </c>
+      <c r="G63">
+        <v>2957.210354943496</v>
+      </c>
+      <c r="H63">
+        <v>10</v>
+      </c>
+      <c r="I63">
+        <v>0</v>
+      </c>
+      <c r="J63">
+        <v>12.61757641792004</v>
+      </c>
+      <c r="K63">
+        <v>11.254056239101089</v>
+      </c>
+      <c r="L63">
+        <v>0.21447520683188909</v>
+      </c>
+      <c r="M63">
+        <v>0.1912979132942568</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>28</v>
+      </c>
+      <c r="B64">
+        <v>27</v>
+      </c>
+      <c r="C64" t="s">
+        <v>20</v>
+      </c>
+      <c r="D64">
+        <v>251.65570919698561</v>
+      </c>
+      <c r="E64">
+        <v>60.397370207276538</v>
+      </c>
+      <c r="F64">
+        <v>41.915774923849924</v>
+      </c>
+      <c r="G64">
+        <v>2963.0675954935969</v>
+      </c>
+      <c r="H64">
+        <v>10</v>
+      </c>
+      <c r="I64">
+        <v>0</v>
+      </c>
+      <c r="J64">
+        <v>11.774291173240311</v>
+      </c>
+      <c r="K64">
+        <v>10.481141113056831</v>
+      </c>
+      <c r="L64">
+        <v>0.24016912133075599</v>
+      </c>
+      <c r="M64">
+        <v>0.21379176161258201</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>28</v>
+      </c>
+      <c r="B65">
+        <v>28</v>
+      </c>
+      <c r="C65" t="s">
+        <v>21</v>
+      </c>
+      <c r="D65">
+        <v>269.27503525084558</v>
+      </c>
+      <c r="E65">
+        <v>64.626008460202939</v>
+      </c>
+      <c r="F65">
+        <v>44.850449871380832</v>
+      </c>
+      <c r="G65">
+        <v>2969.1648750043551</v>
+      </c>
+      <c r="H65">
+        <v>10</v>
+      </c>
+      <c r="I65">
+        <v>0</v>
+      </c>
+      <c r="J65">
+        <v>11.02651373618205</v>
+      </c>
+      <c r="K65">
+        <v>9.7953343411240628</v>
+      </c>
+      <c r="L65">
+        <v>0.26240216268323718</v>
+      </c>
+      <c r="M65">
+        <v>0.2331033159539968</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>29</v>
+      </c>
+      <c r="B66">
+        <v>29</v>
+      </c>
+      <c r="C66" t="s">
+        <v>14</v>
+      </c>
+      <c r="D66">
+        <v>278.30732112667232</v>
+      </c>
+      <c r="E66">
+        <v>66.793757070401369</v>
+      </c>
+      <c r="F66">
+        <v>46.354867406858553</v>
+      </c>
+      <c r="G66">
+        <v>2908.9113788985842</v>
+      </c>
+      <c r="H66">
+        <v>10</v>
+      </c>
+      <c r="I66">
+        <v>0</v>
+      </c>
+      <c r="J66">
+        <v>10.4521554342244</v>
+      </c>
+      <c r="K66">
+        <v>9.4774330381322294</v>
+      </c>
+      <c r="L66">
+        <v>0.28426735840147799</v>
+      </c>
+      <c r="M66">
+        <v>0.257757825276416</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>29</v>
+      </c>
+      <c r="B67">
+        <v>30</v>
+      </c>
+      <c r="C67" t="s">
+        <v>15</v>
+      </c>
+      <c r="D67">
+        <v>296.03071406369662</v>
+      </c>
+      <c r="E67">
+        <v>71.047371375287184</v>
+      </c>
+      <c r="F67">
+        <v>49.306875734449306</v>
+      </c>
+      <c r="G67">
+        <v>2913.759394966602</v>
+      </c>
+      <c r="H67">
+        <v>10</v>
+      </c>
+      <c r="I67">
+        <v>0</v>
+      </c>
+      <c r="J67">
+        <v>9.8427604182302897</v>
+      </c>
+      <c r="K67">
+        <v>8.9100180308738572</v>
+      </c>
+      <c r="L67">
+        <v>0.30115534171025882</v>
+      </c>
+      <c r="M67">
+        <v>0.27261656392270828</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>29</v>
+      </c>
+      <c r="B68">
+        <v>29</v>
+      </c>
+      <c r="C68" t="s">
+        <v>16</v>
+      </c>
+      <c r="D68">
+        <v>278.30732112667232</v>
+      </c>
+      <c r="E68">
+        <v>66.793757070401369</v>
+      </c>
+      <c r="F68">
+        <v>46.354867406858553</v>
+      </c>
+      <c r="G68">
+        <v>2908.9113788985842</v>
+      </c>
+      <c r="H68">
+        <v>10</v>
+      </c>
+      <c r="I68">
+        <v>0</v>
+      </c>
+      <c r="J68">
+        <v>10.4521554342244</v>
+      </c>
+      <c r="K68">
+        <v>9.4774330381322294</v>
+      </c>
+      <c r="L68">
+        <v>0.28426735840147799</v>
+      </c>
+      <c r="M68">
+        <v>0.257757825276416</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>29</v>
+      </c>
+      <c r="B69">
+        <v>28</v>
+      </c>
+      <c r="C69" t="s">
+        <v>17</v>
+      </c>
+      <c r="D69">
+        <v>260.89610279544661</v>
+      </c>
+      <c r="E69">
+        <v>62.615064670907167</v>
+      </c>
+      <c r="F69">
+        <v>43.45485488160957</v>
+      </c>
+      <c r="G69">
+        <v>2904.2560634666661</v>
+      </c>
+      <c r="H69">
+        <v>10</v>
+      </c>
+      <c r="I69">
+        <v>0</v>
+      </c>
+      <c r="J69">
+        <v>11.131849162744009</v>
+      </c>
+      <c r="K69">
+        <v>10.10992104419444</v>
+      </c>
+      <c r="L69">
+        <v>0.26490887009759551</v>
+      </c>
+      <c r="M69">
+        <v>0.24058965598966861</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>29</v>
+      </c>
+      <c r="B70">
+        <v>26</v>
+      </c>
+      <c r="C70" t="s">
+        <v>18</v>
+      </c>
+      <c r="D70">
+        <v>226.95323182219511</v>
+      </c>
+      <c r="E70">
+        <v>54.468775637326821</v>
+      </c>
+      <c r="F70">
+        <v>37.801330292304812</v>
+      </c>
+      <c r="G70">
+        <v>2895.4769401036642</v>
+      </c>
+      <c r="H70">
+        <v>10</v>
+      </c>
+      <c r="I70">
+        <v>0</v>
+      </c>
+      <c r="J70">
+        <v>12.75803352459905</v>
+      </c>
+      <c r="K70">
+        <v>11.621949503968461</v>
+      </c>
+      <c r="L70">
+        <v>0.2168627150195315</v>
+      </c>
+      <c r="M70">
+        <v>0.1975514109122655</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>29</v>
+      </c>
+      <c r="B71">
+        <v>26</v>
+      </c>
+      <c r="C71" t="s">
+        <v>19</v>
+      </c>
+      <c r="D71">
+        <v>226.95323182219511</v>
+      </c>
+      <c r="E71">
+        <v>54.468775637326821</v>
+      </c>
+      <c r="F71">
+        <v>37.801330292304812</v>
+      </c>
+      <c r="G71">
+        <v>2895.4769401036642</v>
+      </c>
+      <c r="H71">
+        <v>10</v>
+      </c>
+      <c r="I71">
+        <v>0</v>
+      </c>
+      <c r="J71">
+        <v>12.75803352459905</v>
+      </c>
+      <c r="K71">
+        <v>11.621949503968461</v>
+      </c>
+      <c r="L71">
+        <v>0.2168627150195315</v>
+      </c>
+      <c r="M71">
+        <v>0.1975514109122655</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>29</v>
+      </c>
+      <c r="B72">
+        <v>27</v>
+      </c>
+      <c r="C72" t="s">
+        <v>20</v>
+      </c>
+      <c r="D72">
+        <v>243.78258640524271</v>
+      </c>
+      <c r="E72">
+        <v>58.507820737258243</v>
+      </c>
+      <c r="F72">
+        <v>40.604427591657213</v>
+      </c>
+      <c r="G72">
+        <v>2899.78154866878</v>
+      </c>
+      <c r="H72">
+        <v>10</v>
+      </c>
+      <c r="I72">
+        <v>0</v>
+      </c>
+      <c r="J72">
+        <v>11.89494947702474</v>
+      </c>
+      <c r="K72">
+        <v>10.819636623328879</v>
+      </c>
+      <c r="L72">
+        <v>0.2426302800005036</v>
+      </c>
+      <c r="M72">
+        <v>0.2206963105217514</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>29</v>
+      </c>
+      <c r="B73">
+        <v>28</v>
+      </c>
+      <c r="C73" t="s">
+        <v>21</v>
+      </c>
+      <c r="D73">
+        <v>260.89610279544661</v>
+      </c>
+      <c r="E73">
+        <v>62.615064670907167</v>
+      </c>
+      <c r="F73">
+        <v>43.45485488160957</v>
+      </c>
+      <c r="G73">
+        <v>2904.2560634666661</v>
+      </c>
+      <c r="H73">
+        <v>10</v>
+      </c>
+      <c r="I73">
+        <v>0</v>
+      </c>
+      <c r="J73">
+        <v>11.131849162744009</v>
+      </c>
+      <c r="K73">
+        <v>10.10992104419444</v>
+      </c>
+      <c r="L73">
+        <v>0.26490887009759551</v>
+      </c>
+      <c r="M73">
+        <v>0.24058965598966861</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:M73" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>